<commit_message>
update changes rating to shop
</commit_message>
<xml_diff>
--- a/backup/Book1.xlsx
+++ b/backup/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\skripsi\implementasi excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\project\sirese\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE3B68-45C6-4596-95A4-13C730EF85D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF671FE-CE82-428C-B6CE-C6F782098930}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4320" windowWidth="20400" windowHeight="6885" activeTab="4" xr2:uid="{614B885E-9B6F-4DE7-A859-E959B12E04EB}"/>
+    <workbookView xWindow="0" yWindow="4680" windowWidth="20400" windowHeight="6885" activeTab="4" xr2:uid="{614B885E-9B6F-4DE7-A859-E959B12E04EB}"/>
   </bookViews>
   <sheets>
     <sheet name="bahan" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">konversi2!$K$18:$K$34</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Book1.xlsxTable3_2OS1" hidden="1">Table3_2[OS]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Book1.xlsxTable3_2Type1" hidden="1">Table3_2[Type]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Book1.xlsxTable3_2OS" hidden="1">Table3_2[OS]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Book1.xlsxTable3_2Type" hidden="1">Table3_2[Type]</definedName>
     <definedName name="ExternalData_1" localSheetId="5" hidden="1">perhitungan!$B$5:$AF$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -77,7 +77,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3_2 OS" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Book1.xlsxTable3_2OS1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Book1.xlsxTable3_2OS"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -86,7 +86,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3_2 Type" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Book1.xlsxTable3_2Type1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Book1.xlsxTable3_2Type"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="322">
   <si>
     <t>Merk</t>
   </si>
@@ -1192,6 +1192,9 @@
   <si>
     <t>&gt; 400000</t>
   </si>
+  <si>
+    <t>Bobot Akhir</t>
+  </si>
 </sst>
 </file>
 
@@ -1201,9 +1204,9 @@
     <numFmt numFmtId="44" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$Rp-421]* #,##0.00_-;\-[$Rp-421]* #,##0.00_-;_-[$Rp-421]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1312,6 +1315,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1577,7 +1588,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1752,20 +1763,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1776,11 +1788,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1800,16 +1821,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="15" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1817,136 +1839,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="162">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FF7F7F7F"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="163">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2626,6 +2521,136 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3784,6 +3809,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4755,17 +4848,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F837D00-D370-4A6C-BB62-A90B55009448}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Cipset">
-  <location ref="D19:D25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB64776-FF22-480F-A386-74F63A6BA229}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Screen Type">
+  <location ref="H5:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="1"/>
+        <item x="3"/>
         <item x="4"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -4792,67 +4884,34 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
+  <pivotHierarchies count="5">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="1"/>
+  </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Book1.xlsx!Table3_2[Type]">
+        <x15:activeTabTopLevelEntity name="[Table3_2 Type]"/>
+      </x15:pivotTableUISettings>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E632C48D-E08A-4023-A608-386B5EE4E460}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Main Type">
-  <location ref="H19:H23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{203D94C7-2432-488D-A184-891F6ADA82EE}" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="OS">
   <location ref="J5:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
@@ -4903,6 +4962,47 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{83EEB2CE-8A5E-44D4-93F7-D7801FB551A6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="build Back">
+  <location ref="F5:F8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -5049,16 +5149,17 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADB64776-FF22-480F-A386-74F63A6BA229}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Screen Type">
-  <location ref="H5:H11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F837D00-D370-4A6C-BB62-A90B55009448}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Cipset">
+  <location ref="D19:D25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
         <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
+        <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -5085,41 +5186,30 @@
       <x/>
     </i>
   </rowItems>
-  <pivotHierarchies count="5">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-  </pivotHierarchies>
+  <colItems count="1">
+    <i/>
+  </colItems>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="1"/>
-  </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_Book1.xlsx!Table3_2[Type]">
-        <x15:activeTabTopLevelEntity name="[Table3_2 Type]"/>
-      </x15:pivotTableUISettings>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{83EEB2CE-8A5E-44D4-93F7-D7801FB551A6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="build Back">
-  <location ref="F5:F8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E632C48D-E08A-4023-A608-386B5EE4E460}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Main Type">
+  <location ref="H19:H23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" showAll="0">
-      <items count="3">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
         <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5127,12 +5217,15 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -5194,49 +5287,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A843DCF4-43D7-4723-A8ED-2AB029E4DF31}" name="Table3" displayName="Table3" ref="B19:AB47" totalsRowShown="0" headerRowDxfId="161" dataDxfId="159" headerRowBorderDxfId="160" tableBorderDxfId="158" totalsRowBorderDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A843DCF4-43D7-4723-A8ED-2AB029E4DF31}" name="Table3" displayName="Table3" ref="B19:AB47" totalsRowShown="0" headerRowDxfId="162" dataDxfId="160" headerRowBorderDxfId="161" tableBorderDxfId="159" totalsRowBorderDxfId="158">
   <autoFilter ref="B19:AB47" xr:uid="{432B4ABB-9276-4950-A6C9-9543288073C7}"/>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{CD6D49EC-35F7-4F52-82BE-628647EE31D4}" name="Brand" dataDxfId="156"/>
-    <tableColumn id="2" xr3:uid="{202BE39B-0490-444B-B1F0-8DE33922156B}" name="Merk" dataDxfId="155"/>
-    <tableColumn id="3" xr3:uid="{E3EFE68F-0723-4EF1-ABF2-3C99AD7B861A}" name="Dimension" dataDxfId="154"/>
-    <tableColumn id="4" xr3:uid="{9CF0F0EA-FFF6-47A3-9805-5C240464ECB7}" name="Weight" dataDxfId="153"/>
-    <tableColumn id="5" xr3:uid="{FC68040B-3CD9-4204-A50A-FF596C23CE43}" name="build" dataDxfId="152"/>
-    <tableColumn id="6" xr3:uid="{F11135C7-9E8B-4BDB-9193-94ECFFB815F9}" name="Dual SIM" dataDxfId="151"/>
-    <tableColumn id="7" xr3:uid="{8489B171-391B-450B-8BB5-4F4D27EB1848}" name="5G" dataDxfId="150"/>
-    <tableColumn id="8" xr3:uid="{B27D4B2F-9D60-408B-B20C-BC20B819DD70}" name="Type" dataDxfId="149"/>
-    <tableColumn id="9" xr3:uid="{EC5EEEFA-1CE0-4E18-9A7E-1C25A1990C6B}" name="Size" dataDxfId="148"/>
-    <tableColumn id="10" xr3:uid="{90141041-D52E-40BA-BE3A-B3986163947A}" name="Resolution" dataDxfId="147"/>
-    <tableColumn id="11" xr3:uid="{87359EAF-281C-4F61-9926-99665D1A63E5}" name="OS" dataDxfId="146"/>
-    <tableColumn id="12" xr3:uid="{D8C1C070-CF5C-4CA2-9145-26F8DAD27B18}" name="Chipset" dataDxfId="145"/>
-    <tableColumn id="13" xr3:uid="{2D6204CB-5718-4ECC-A87B-D087CF177FCB}" name="CPU" dataDxfId="144"/>
-    <tableColumn id="14" xr3:uid="{6E5DC8CF-2459-471C-8B89-272F98E2DC0D}" name="Card Slot" dataDxfId="143"/>
-    <tableColumn id="15" xr3:uid="{63CBFABA-2D16-4296-BE61-E0E51EDC7B3C}" name="RAM" dataDxfId="142"/>
-    <tableColumn id="16" xr3:uid="{A21A9336-3992-4646-B290-5AF7015E6EFF}" name="ROM" dataDxfId="141"/>
-    <tableColumn id="17" xr3:uid="{785B3860-44A8-4BED-8CBC-8C3EF3994AF9}" name="Camera" dataDxfId="140"/>
-    <tableColumn id="18" xr3:uid="{586FF55C-D7FF-45D6-9DBB-21C8D70B4B37}" name="Type2" dataDxfId="139"/>
-    <tableColumn id="19" xr3:uid="{D315ACE9-1535-49B1-8B22-500E6239AB51}" name="Video" dataDxfId="138"/>
-    <tableColumn id="20" xr3:uid="{8103FBE4-39F7-445D-8CDF-6C7E841EE7F0}" name="Camera3" dataDxfId="137"/>
-    <tableColumn id="21" xr3:uid="{EA52EBB1-40FB-4122-BF26-75B8D9D8A069}" name="Type4" dataDxfId="136"/>
-    <tableColumn id="22" xr3:uid="{7323E3D6-1A5E-4F3B-B09D-2488C115446B}" name="Video2" dataDxfId="135"/>
-    <tableColumn id="23" xr3:uid="{A782E266-68D4-43CF-8852-2272263883EA}" name="USB" dataDxfId="134"/>
-    <tableColumn id="24" xr3:uid="{EE14A4F6-5B40-432D-BF5E-411BB7EA90FA}" name="Capacity" dataDxfId="133"/>
-    <tableColumn id="25" xr3:uid="{37E34D68-AEE6-4808-B33D-922C3E02B2F4}" name="Type6" dataDxfId="132"/>
-    <tableColumn id="26" xr3:uid="{1CC14D51-432E-47CE-AC2B-F81B871D036C}" name="Wireless" dataDxfId="131"/>
-    <tableColumn id="27" xr3:uid="{EA0027F3-B2B5-4CC9-B528-2EE7E248FF32}" name="Price" dataDxfId="130" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{CD6D49EC-35F7-4F52-82BE-628647EE31D4}" name="Brand" dataDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{202BE39B-0490-444B-B1F0-8DE33922156B}" name="Merk" dataDxfId="156"/>
+    <tableColumn id="3" xr3:uid="{E3EFE68F-0723-4EF1-ABF2-3C99AD7B861A}" name="Dimension" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{9CF0F0EA-FFF6-47A3-9805-5C240464ECB7}" name="Weight" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{FC68040B-3CD9-4204-A50A-FF596C23CE43}" name="build" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{F11135C7-9E8B-4BDB-9193-94ECFFB815F9}" name="Dual SIM" dataDxfId="152"/>
+    <tableColumn id="7" xr3:uid="{8489B171-391B-450B-8BB5-4F4D27EB1848}" name="5G" dataDxfId="151"/>
+    <tableColumn id="8" xr3:uid="{B27D4B2F-9D60-408B-B20C-BC20B819DD70}" name="Type" dataDxfId="150"/>
+    <tableColumn id="9" xr3:uid="{EC5EEEFA-1CE0-4E18-9A7E-1C25A1990C6B}" name="Size" dataDxfId="149"/>
+    <tableColumn id="10" xr3:uid="{90141041-D52E-40BA-BE3A-B3986163947A}" name="Resolution" dataDxfId="148"/>
+    <tableColumn id="11" xr3:uid="{87359EAF-281C-4F61-9926-99665D1A63E5}" name="OS" dataDxfId="147"/>
+    <tableColumn id="12" xr3:uid="{D8C1C070-CF5C-4CA2-9145-26F8DAD27B18}" name="Chipset" dataDxfId="146"/>
+    <tableColumn id="13" xr3:uid="{2D6204CB-5718-4ECC-A87B-D087CF177FCB}" name="CPU" dataDxfId="145"/>
+    <tableColumn id="14" xr3:uid="{6E5DC8CF-2459-471C-8B89-272F98E2DC0D}" name="Card Slot" dataDxfId="144"/>
+    <tableColumn id="15" xr3:uid="{63CBFABA-2D16-4296-BE61-E0E51EDC7B3C}" name="RAM" dataDxfId="143"/>
+    <tableColumn id="16" xr3:uid="{A21A9336-3992-4646-B290-5AF7015E6EFF}" name="ROM" dataDxfId="142"/>
+    <tableColumn id="17" xr3:uid="{785B3860-44A8-4BED-8CBC-8C3EF3994AF9}" name="Camera" dataDxfId="141"/>
+    <tableColumn id="18" xr3:uid="{586FF55C-D7FF-45D6-9DBB-21C8D70B4B37}" name="Type2" dataDxfId="140"/>
+    <tableColumn id="19" xr3:uid="{D315ACE9-1535-49B1-8B22-500E6239AB51}" name="Video" dataDxfId="139"/>
+    <tableColumn id="20" xr3:uid="{8103FBE4-39F7-445D-8CDF-6C7E841EE7F0}" name="Camera3" dataDxfId="138"/>
+    <tableColumn id="21" xr3:uid="{EA52EBB1-40FB-4122-BF26-75B8D9D8A069}" name="Type4" dataDxfId="137"/>
+    <tableColumn id="22" xr3:uid="{7323E3D6-1A5E-4F3B-B09D-2488C115446B}" name="Video2" dataDxfId="136"/>
+    <tableColumn id="23" xr3:uid="{A782E266-68D4-43CF-8852-2272263883EA}" name="USB" dataDxfId="135"/>
+    <tableColumn id="24" xr3:uid="{EE14A4F6-5B40-432D-BF5E-411BB7EA90FA}" name="Capacity" dataDxfId="134"/>
+    <tableColumn id="25" xr3:uid="{37E34D68-AEE6-4808-B33D-922C3E02B2F4}" name="Type6" dataDxfId="133"/>
+    <tableColumn id="26" xr3:uid="{1CC14D51-432E-47CE-AC2B-F81B871D036C}" name="Wireless" dataDxfId="132"/>
+    <tableColumn id="27" xr3:uid="{EA0027F3-B2B5-4CC9-B528-2EE7E248FF32}" name="Price" dataDxfId="131" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0A0FA78B-E872-4658-9773-C43E07BEBD9A}" name="Table7" displayName="Table7" ref="C5:F14" totalsRowShown="0" headerRowDxfId="129" dataDxfId="127" headerRowBorderDxfId="128" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0A0FA78B-E872-4658-9773-C43E07BEBD9A}" name="Table7" displayName="Table7" ref="C5:F14" totalsRowShown="0" headerRowDxfId="130" dataDxfId="128" headerRowBorderDxfId="129" tableBorderDxfId="127">
   <autoFilter ref="C5:F14" xr:uid="{D0CE1693-3C37-4A41-9171-8A805A47437A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{84FC2797-FF0E-4C60-96B4-E401AC99B3B3}" name="No" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{F38BACFE-A358-40A8-9676-26C3AB98220C}" name="Kriteria" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{51D43D22-25AF-4A78-9EBC-43BEC07B468E}" name="Bobot" dataDxfId="123"/>
-    <tableColumn id="4" xr3:uid="{3AFEBD26-BD4F-4B41-B893-1F757253C6B9}" name="Normalisasi" dataDxfId="122">
+    <tableColumn id="1" xr3:uid="{84FC2797-FF0E-4C60-96B4-E401AC99B3B3}" name="No" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{F38BACFE-A358-40A8-9676-26C3AB98220C}" name="Kriteria" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{51D43D22-25AF-4A78-9EBC-43BEC07B468E}" name="Bobot" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{3AFEBD26-BD4F-4B41-B893-1F757253C6B9}" name="Normalisasi" dataDxfId="123">
       <calculatedColumnFormula>SUM(E6/$E$15)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5245,53 +5338,56 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{261173BA-8F57-49A8-BFB1-52BAA8678DFE}" name="Table710" displayName="Table710" ref="I5:L13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
-  <autoFilter ref="I5:L13" xr:uid="{34406045-360A-4D16-803D-10A85ED8ED8D}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F4B08FF-4448-4A8D-9E03-A0951E9D0085}" name="No" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{6358A033-0215-47D8-9411-97C96313F1B2}" name="Kriteria" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{E1F21746-C1E7-4F35-B37B-29675E169DA1}" name="Bobot" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{2333B1F6-2EC6-4C5B-8F33-2EE0B8087C5F}" name="Normalisasi" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{261173BA-8F57-49A8-BFB1-52BAA8678DFE}" name="Table710" displayName="Table710" ref="I5:M13" totalsRowShown="0" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121" tableBorderDxfId="119">
+  <autoFilter ref="I5:M13" xr:uid="{34406045-360A-4D16-803D-10A85ED8ED8D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7F4B08FF-4448-4A8D-9E03-A0951E9D0085}" name="No" dataDxfId="118" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{6358A033-0215-47D8-9411-97C96313F1B2}" name="Kriteria" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{E1F21746-C1E7-4F35-B37B-29675E169DA1}" name="Bobot" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{2333B1F6-2EC6-4C5B-8F33-2EE0B8087C5F}" name="Normalisasi" dataDxfId="115">
       <calculatedColumnFormula>SUM(K6/$K$14)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" xr3:uid="{8248D30E-1BF8-4D68-874F-D37DFD3A4606}" name="Bobot Akhir" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>L6</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14AE9411-2E5B-4909-A723-2DCA54A1AFE6}" name="Table3_2" displayName="Table3_2" ref="B5:AF33" tableType="queryTable" totalsRowShown="0" headerRowDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14AE9411-2E5B-4909-A723-2DCA54A1AFE6}" name="Table3_2" displayName="Table3_2" ref="B5:AF33" tableType="queryTable" totalsRowShown="0" headerRowDxfId="114">
   <autoFilter ref="B5:AF33" xr:uid="{AE2678E8-9A8C-4036-BA05-73E5B497A284}"/>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{7BC2F3AC-BE12-4340-B3E5-ABFA3687F5BE}" uniqueName="1" name="Brand" queryTableFieldId="1" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{7BC2F3AC-BE12-4340-B3E5-ABFA3687F5BE}" uniqueName="1" name="Brand" queryTableFieldId="1" dataDxfId="113"/>
     <tableColumn id="2" xr3:uid="{D81010F7-B063-4609-9DB8-FE8E1B38460A}" uniqueName="2" name="Merk" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{A0538A90-8D15-4CE2-BBA0-01BFB16EF250}" uniqueName="3" name="Dimension.1" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{9A32168D-F70A-42E2-B8A9-EA260A7FA180}" uniqueName="4" name="Dimension.3" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{B22AF4FA-A3D2-4F23-92B4-B5985D65DC5D}" uniqueName="5" name="Dimension.5" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{B17C9FF9-02B3-4352-99DC-B0E28E42811F}" uniqueName="6" name="Weight.1" queryTableFieldId="6" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{3BE0FDAE-A1DA-45A7-B21B-97088ACF7243}" uniqueName="7" name="build.2" queryTableFieldId="7" dataDxfId="118"/>
-    <tableColumn id="8" xr3:uid="{C4F0A00C-3712-4B98-8AAE-442675A36F7E}" uniqueName="8" name="build.3" queryTableFieldId="8" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{B17C9FF9-02B3-4352-99DC-B0E28E42811F}" uniqueName="6" name="Weight.1" queryTableFieldId="6" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{3BE0FDAE-A1DA-45A7-B21B-97088ACF7243}" uniqueName="7" name="build.2" queryTableFieldId="7" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{C4F0A00C-3712-4B98-8AAE-442675A36F7E}" uniqueName="8" name="build.3" queryTableFieldId="8" dataDxfId="110"/>
     <tableColumn id="9" xr3:uid="{4A32AB7F-60BC-49FA-9791-9C5B61CE8000}" uniqueName="9" name="Type" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{5FB29773-E321-47C2-ACB2-3855FBD04F69}" uniqueName="10" name="Size.1" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{1B771B9E-5988-4470-B4CE-FADC83ADA4C8}" uniqueName="11" name="Resolution.1" queryTableFieldId="11"/>
-    <tableColumn id="12" xr3:uid="{40CF70A0-08BD-4364-BA1B-1AD5AD2B6543}" uniqueName="12" name="Resolution.2" queryTableFieldId="12" dataDxfId="116"/>
-    <tableColumn id="13" xr3:uid="{B4D598AB-BD80-49E1-B935-7482BA49D815}" uniqueName="13" name="OS" queryTableFieldId="13" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{812E202C-3C4B-4C33-825B-5CA5A42D2B9E}" uniqueName="14" name="Chipset" queryTableFieldId="14" dataDxfId="114"/>
+    <tableColumn id="12" xr3:uid="{40CF70A0-08BD-4364-BA1B-1AD5AD2B6543}" uniqueName="12" name="Resolution.2" queryTableFieldId="12" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{B4D598AB-BD80-49E1-B935-7482BA49D815}" uniqueName="13" name="OS" queryTableFieldId="13" dataDxfId="108"/>
+    <tableColumn id="14" xr3:uid="{812E202C-3C4B-4C33-825B-5CA5A42D2B9E}" uniqueName="14" name="Chipset" queryTableFieldId="14" dataDxfId="107"/>
     <tableColumn id="15" xr3:uid="{D8DA605D-4FC8-47C4-A1A4-E0CAC3F14212}" uniqueName="15" name="CPU" queryTableFieldId="15"/>
     <tableColumn id="16" xr3:uid="{C03599F2-C5DA-4BCC-A50A-367CA59939F6}" uniqueName="16" name="RAM" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{97CC3950-D19F-4388-B58F-F221627A5AF9}" uniqueName="17" name="ROM" queryTableFieldId="17" dataDxfId="113"/>
-    <tableColumn id="18" xr3:uid="{CC78B974-3AF2-4311-93F2-8F35B9DA50DA}" uniqueName="18" name="Camera" queryTableFieldId="18" dataDxfId="112"/>
-    <tableColumn id="19" xr3:uid="{0F924B9F-FDD2-4081-BF9E-6294EA39A3B8}" uniqueName="19" name="Type2" queryTableFieldId="19" dataDxfId="111"/>
-    <tableColumn id="20" xr3:uid="{A6071C53-DC01-4A6C-B44D-786626D65382}" uniqueName="20" name="Video.1" queryTableFieldId="20" dataDxfId="110"/>
-    <tableColumn id="21" xr3:uid="{8F5BDFA3-AA39-4A67-AD9E-555E25EBCBAC}" uniqueName="21" name="Video.2" queryTableFieldId="21" dataDxfId="109"/>
-    <tableColumn id="22" xr3:uid="{EB699D74-1417-46F8-8FE0-5CDE60349482}" uniqueName="22" name="Video.3" queryTableFieldId="22" dataDxfId="108"/>
-    <tableColumn id="23" xr3:uid="{A8CB5DBE-130B-480B-97B2-D1E5124269C2}" uniqueName="23" name="Video.4" queryTableFieldId="23" dataDxfId="107"/>
-    <tableColumn id="24" xr3:uid="{B56D0E94-83F1-421F-B679-AA6D8EA66BEF}" uniqueName="24" name="Camera3" queryTableFieldId="24" dataDxfId="106"/>
-    <tableColumn id="25" xr3:uid="{CC14FFCB-8106-49F1-9ADD-2565626B5082}" uniqueName="25" name="Type4" queryTableFieldId="25" dataDxfId="105"/>
-    <tableColumn id="26" xr3:uid="{24550311-39D1-41B3-832F-BC9AB8DDCA73}" uniqueName="26" name="Video2.1" queryTableFieldId="26" dataDxfId="104"/>
-    <tableColumn id="27" xr3:uid="{A78D7702-46E4-4DFC-88F4-1B02CC570ECB}" uniqueName="27" name="Video2.2" queryTableFieldId="27" dataDxfId="103"/>
-    <tableColumn id="28" xr3:uid="{A54E068F-D679-4E17-BE37-8D6050C229B6}" uniqueName="28" name="USB" queryTableFieldId="28" dataDxfId="102"/>
-    <tableColumn id="29" xr3:uid="{C3263A92-6EF2-40A9-9A36-0C45BD705D2E}" uniqueName="29" name="Capacity" queryTableFieldId="29" dataDxfId="101"/>
+    <tableColumn id="17" xr3:uid="{97CC3950-D19F-4388-B58F-F221627A5AF9}" uniqueName="17" name="ROM" queryTableFieldId="17" dataDxfId="106"/>
+    <tableColumn id="18" xr3:uid="{CC78B974-3AF2-4311-93F2-8F35B9DA50DA}" uniqueName="18" name="Camera" queryTableFieldId="18" dataDxfId="105"/>
+    <tableColumn id="19" xr3:uid="{0F924B9F-FDD2-4081-BF9E-6294EA39A3B8}" uniqueName="19" name="Type2" queryTableFieldId="19" dataDxfId="104"/>
+    <tableColumn id="20" xr3:uid="{A6071C53-DC01-4A6C-B44D-786626D65382}" uniqueName="20" name="Video.1" queryTableFieldId="20" dataDxfId="103"/>
+    <tableColumn id="21" xr3:uid="{8F5BDFA3-AA39-4A67-AD9E-555E25EBCBAC}" uniqueName="21" name="Video.2" queryTableFieldId="21" dataDxfId="102"/>
+    <tableColumn id="22" xr3:uid="{EB699D74-1417-46F8-8FE0-5CDE60349482}" uniqueName="22" name="Video.3" queryTableFieldId="22" dataDxfId="101"/>
+    <tableColumn id="23" xr3:uid="{A8CB5DBE-130B-480B-97B2-D1E5124269C2}" uniqueName="23" name="Video.4" queryTableFieldId="23" dataDxfId="100"/>
+    <tableColumn id="24" xr3:uid="{B56D0E94-83F1-421F-B679-AA6D8EA66BEF}" uniqueName="24" name="Camera3" queryTableFieldId="24" dataDxfId="99"/>
+    <tableColumn id="25" xr3:uid="{CC14FFCB-8106-49F1-9ADD-2565626B5082}" uniqueName="25" name="Type4" queryTableFieldId="25" dataDxfId="98"/>
+    <tableColumn id="26" xr3:uid="{24550311-39D1-41B3-832F-BC9AB8DDCA73}" uniqueName="26" name="Video2.1" queryTableFieldId="26" dataDxfId="97"/>
+    <tableColumn id="27" xr3:uid="{A78D7702-46E4-4DFC-88F4-1B02CC570ECB}" uniqueName="27" name="Video2.2" queryTableFieldId="27" dataDxfId="96"/>
+    <tableColumn id="28" xr3:uid="{A54E068F-D679-4E17-BE37-8D6050C229B6}" uniqueName="28" name="USB" queryTableFieldId="28" dataDxfId="95"/>
+    <tableColumn id="29" xr3:uid="{C3263A92-6EF2-40A9-9A36-0C45BD705D2E}" uniqueName="29" name="Capacity" queryTableFieldId="29" dataDxfId="94"/>
     <tableColumn id="30" xr3:uid="{0680B8DC-A1EC-4234-BE5A-18AA4E356B6F}" uniqueName="30" name="Type6" queryTableFieldId="30"/>
     <tableColumn id="31" xr3:uid="{EDB5532F-71A2-4862-BAF7-E80ED2EA7BCF}" uniqueName="31" name="Price" queryTableFieldId="31"/>
   </tableColumns>
@@ -5300,70 +5396,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CFC4B63-5A5A-4A8C-880A-0D71DA3C0CE4}" name="Table2" displayName="Table2" ref="B37:V65" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CFC4B63-5A5A-4A8C-880A-0D71DA3C0CE4}" name="Table2" displayName="Table2" ref="B37:V65" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="B37:V65" xr:uid="{64E79E36-124F-4C27-93BF-57235FBA513B}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{B1193B3A-F98F-40C9-AE76-51ADA415328C}" name="Brand" dataDxfId="98">
+    <tableColumn id="1" xr3:uid="{B1193B3A-F98F-40C9-AE76-51ADA415328C}" name="Brand" dataDxfId="91">
       <calculatedColumnFormula>IF(B6='normalisasi data'!$E$3,'normalisasi data'!$E$14,IF(perhitungan!B6='normalisasi data'!$F$3,'normalisasi data'!$F$14,IF(perhitungan!B6='normalisasi data'!$G$3,'normalisasi data'!$G$14,"null")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5C1EBBFC-0C07-4E1B-A260-3129923096BE}" name="Merek" dataDxfId="97">
+    <tableColumn id="2" xr3:uid="{5C1EBBFC-0C07-4E1B-A260-3129923096BE}" name="Merek" dataDxfId="90">
       <calculatedColumnFormula>C6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC6DA604-3E46-420E-B778-AA812E6B0E39}" name="Dimensi" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{EC6DA604-3E46-420E-B778-AA812E6B0E39}" name="Dimensi" dataDxfId="89">
       <calculatedColumnFormula>SUM(D6*E6*F6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AD7440B1-BC17-4DE7-8DE1-B6791979323F}" name="Berat" dataDxfId="95">
+    <tableColumn id="4" xr3:uid="{AD7440B1-BC17-4DE7-8DE1-B6791979323F}" name="Berat" dataDxfId="88">
       <calculatedColumnFormula>G6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF9A45BE-9C65-4870-9381-7F2A53EEB9E0}" name="Build" dataDxfId="94">
+    <tableColumn id="5" xr3:uid="{CF9A45BE-9C65-4870-9381-7F2A53EEB9E0}" name="Build" dataDxfId="87">
       <calculatedColumnFormula>IF(H6=konversi!$D$6,konversi!$E$6,IF(perhitungan!H6=konversi!$D$7,konversi!$E$7,0))+IF(I6=konversi!$F$6,konversi!$G$6,IF(perhitungan!I6=konversi!$F$7,konversi!$G$7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A6978DC-F0E6-4A66-A0BC-817A62D4A3B7}" name="Type Layar" dataDxfId="93">
+    <tableColumn id="7" xr3:uid="{4A6978DC-F0E6-4A66-A0BC-817A62D4A3B7}" name="Type Layar" dataDxfId="86">
       <calculatedColumnFormula>IF(J6=konversi!$H$6,konversi!$I$6,IF(perhitungan!J6=konversi!$H$7,konversi!$I$7,IF(perhitungan!J6=konversi!$H$8,konversi!$I$8,IF(perhitungan!J6=konversi!$H$9,konversi!I8,IF(perhitungan!J6=konversi!$H$10,konversi!$I$10,"null")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D2EB4666-92EA-48DD-9D69-40784758D291}" name="Ukuran Layar" dataDxfId="92">
+    <tableColumn id="8" xr3:uid="{D2EB4666-92EA-48DD-9D69-40784758D291}" name="Ukuran Layar" dataDxfId="85">
       <calculatedColumnFormula>K6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4DF057B4-E7B3-4564-B89B-A5C7D1746468}" name="Resolusi" dataDxfId="91">
+    <tableColumn id="9" xr3:uid="{4DF057B4-E7B3-4564-B89B-A5C7D1746468}" name="Resolusi" dataDxfId="84">
       <calculatedColumnFormula>SUM(L6*M6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3F64312E-CBA2-4B15-A292-2754A87DF648}" name="OS" dataDxfId="90">
+    <tableColumn id="10" xr3:uid="{3F64312E-CBA2-4B15-A292-2754A87DF648}" name="OS" dataDxfId="83">
       <calculatedColumnFormula>IF(N6=konversi!$J$6,konversi!$K$6,IF(perhitungan!N6=konversi!$J$7,konversi!$K$7,IF(perhitungan!N6=konversi!$J$8,konversi!$K$8,"null")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CE5ECF8A-9C8D-4263-8844-D0ACE47C39FE}" name="Chipset" dataDxfId="89">
+    <tableColumn id="11" xr3:uid="{CE5ECF8A-9C8D-4263-8844-D0ACE47C39FE}" name="Chipset" dataDxfId="82">
       <calculatedColumnFormula>IF(perhitungan!O6=konversi!$D$20,konversi!$E$20,IF(perhitungan!O6=konversi!$D$21,konversi!$E$21,IF(perhitungan!O6=konversi!$D$22,konversi!$E$22,IF(perhitungan!O6=konversi!$D$23,konversi!$E$23,IF(perhitungan!O6=konversi!$D$24,konversi!$E$24,"null")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{84760D73-4328-44A2-A11C-F5033D6F190A}" name="CPU" dataDxfId="88">
+    <tableColumn id="12" xr3:uid="{84760D73-4328-44A2-A11C-F5033D6F190A}" name="CPU" dataDxfId="81">
       <calculatedColumnFormula>IF(P6=konversi!$F$20,konversi!$G$20,IF(perhitungan!P6=konversi!$F$21,konversi!$G$21,IF(perhitungan!P6=konversi!$F$22,konversi!$G$22,"null")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{162D8D16-0758-4950-B1CD-84D318ABED1A}" name="RAM" dataDxfId="87">
+    <tableColumn id="13" xr3:uid="{162D8D16-0758-4950-B1CD-84D318ABED1A}" name="RAM" dataDxfId="80">
       <calculatedColumnFormula>Q6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{63FFA25A-D557-4C84-8A37-19299CED9659}" name="ROM" dataDxfId="86">
+    <tableColumn id="14" xr3:uid="{63FFA25A-D557-4C84-8A37-19299CED9659}" name="ROM" dataDxfId="79">
       <calculatedColumnFormula>R6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{397749AE-83C6-4AB2-AA06-AC77A7F94708}" name="MP Main" dataDxfId="85">
+    <tableColumn id="15" xr3:uid="{397749AE-83C6-4AB2-AA06-AC77A7F94708}" name="MP Main" dataDxfId="78">
       <calculatedColumnFormula>S6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{6A466ED6-412F-436A-A21B-D53290D381A8}" name="Tipe Main" dataDxfId="84">
+    <tableColumn id="16" xr3:uid="{6A466ED6-412F-436A-A21B-D53290D381A8}" name="Tipe Main" dataDxfId="77">
       <calculatedColumnFormula>IF(T6=konversi!$H$20,konversi!$I$20,IF(perhitungan!T6=konversi!$H$21,konversi!$I$21,IF(perhitungan!T6=konversi!$H$22,konversi!$I$22,"null")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{0DA2F041-432A-4DAB-83D2-CA057A26E65A}" name="Video Main" dataDxfId="83">
+    <tableColumn id="17" xr3:uid="{0DA2F041-432A-4DAB-83D2-CA057A26E65A}" name="Video Main" dataDxfId="76">
       <calculatedColumnFormula>IF(perhitungan!U6=konversi!$B$32,konversi!$C$32,IF(perhitungan!U6=konversi!$B$33,konversi!$C$33,IF(perhitungan!U6=konversi!$B$34,konversi!$C$34,IF(perhitungan!U6=konversi!$B$35,konversi!$C$35,IF(perhitungan!U6=konversi!$B$36,konversi!$C$36,IF(perhitungan!U6=konversi!$B$37,konversi!$C$37,IF(perhitungan!U6=konversi!$B$38,konversi!$C$38,0))))))) + IF(perhitungan!V6=konversi!$B$32,konversi!$C$32,IF(perhitungan!V6=konversi!$B$33,konversi!$C$33,IF(perhitungan!V6=konversi!$B$34,konversi!$C$34,IF(perhitungan!V6=konversi!$B$35,konversi!$C$35,IF(perhitungan!U6=konversi!$B$36,konversi!$C$36,IF(perhitungan!V6=konversi!$B$37,konversi!$C$37,IF(perhitungan!V6=konversi!$B$38,konversi!$C$38,0)))))))  + IF(perhitungan!W6=konversi!$B$32,konversi!$C$32,IF(perhitungan!W6=konversi!$B$33,konversi!$C$33,IF(perhitungan!W6=konversi!$B$34,konversi!$C$34,IF(perhitungan!W6=konversi!$B$35,konversi!$C$35,IF(perhitungan!W6=konversi!$B$36,konversi!$C$36,IF(perhitungan!W6=konversi!$B$37,konversi!$C$37,IF(perhitungan!W6=konversi!$B$38,konversi!$C$38,0)))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{A4DA33AF-1EF9-472D-A57F-59D6DC0BA712}" name="MP Front" dataDxfId="82">
+    <tableColumn id="18" xr3:uid="{A4DA33AF-1EF9-472D-A57F-59D6DC0BA712}" name="MP Front" dataDxfId="75">
       <calculatedColumnFormula>Y6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{A3831012-701E-40F1-8FBC-584C96096E0C}" name="Video Front" dataDxfId="81">
+    <tableColumn id="20" xr3:uid="{A3831012-701E-40F1-8FBC-584C96096E0C}" name="Video Front" dataDxfId="74">
       <calculatedColumnFormula>IF(AA6=konversi!$H$28,konversi!$I$28,IF(AA6=konversi!$H$29,konversi!$I$29,IF(AA6=konversi!$H$30,konversi!$I$30,IF(AA6=konversi!$H$31,konversi!$I$31,IF(AA6=konversi!$H$32,konversi!$I$32,IF(AA6=konversi!$H$33,konversi!$I$33,IF(AA6=konversi!$H$34,konversi!$I$34,0))))))) + IF(AB6=konversi!$H$28,konversi!$I$28,IF(AB6=konversi!$H$29,konversi!$I$29,IF(AB6=konversi!$H$30,konversi!$I$30,IF(AB6=konversi!$H$31,konversi!$I$31,IF(AB6=konversi!$H$32,konversi!$I$32,IF(AB6=konversi!$H$33,konversi!$I$33,IF(AB6=konversi!$H$34,konversi!$I$34,0)))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{32E5E990-3ABF-4966-B40F-F63ACCFBB99A}" name="USB Type" dataDxfId="80">
+    <tableColumn id="21" xr3:uid="{32E5E990-3ABF-4966-B40F-F63ACCFBB99A}" name="USB Type" dataDxfId="73">
       <calculatedColumnFormula>IF(AC6=konversi!$D$33,konversi!$E$33,IF(AC6=konversi!$D$34,konversi!$E$34,IF(AC6=konversi!$D$35,konversi!$E$35,IF(AC6=konversi!$D$36,konversi!$E$36,IF(AC6=konversi!$D$37,konversi!$E$37,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{1E48D67D-06B2-485A-AD0A-FB484ADE6C62}" name="Capacity" dataDxfId="79">
+    <tableColumn id="22" xr3:uid="{1E48D67D-06B2-485A-AD0A-FB484ADE6C62}" name="Capacity" dataDxfId="72">
       <calculatedColumnFormula>AD6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{6844A1B9-D904-4D72-94CE-9A607EBC6CA1}" name="Harga" dataDxfId="78">
+    <tableColumn id="24" xr3:uid="{6844A1B9-D904-4D72-94CE-9A607EBC6CA1}" name="Harga" dataDxfId="71">
       <calculatedColumnFormula>AF6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5376,67 +5472,67 @@
   <autoFilter ref="A107:V135" xr:uid="{B7713168-1958-4E1B-9B04-826311F8B811}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{BBD7E74A-EF79-4D26-8688-12FB791727AE}" name="No"/>
-    <tableColumn id="2" xr3:uid="{19EE6246-ADF8-44BB-8377-76B0A218E33C}" name="Brand" dataDxfId="77">
+    <tableColumn id="2" xr3:uid="{19EE6246-ADF8-44BB-8377-76B0A218E33C}" name="Brand" dataDxfId="70">
       <calculatedColumnFormula>SUM(((B70 - MIN(Table2[Brand]))/(MAX(Table2[Brand]) - MIN(Table2[Brand]))) *100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FB26A1BE-D228-466F-887F-71A725852FDE}" name="Merek" dataDxfId="76">
+    <tableColumn id="3" xr3:uid="{FB26A1BE-D228-466F-887F-71A725852FDE}" name="Merek" dataDxfId="69">
       <calculatedColumnFormula>C38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DA20BE13-BC08-4CC7-BF50-104E7C385BF2}" name="Dimensi" dataDxfId="75">
+    <tableColumn id="4" xr3:uid="{DA20BE13-BC08-4CC7-BF50-104E7C385BF2}" name="Dimensi" dataDxfId="68">
       <calculatedColumnFormula>SUM(((D70-MIN(Table4[Dimensi]))/(MAX(Table4[Dimensi])-MIN(Table4[Dimensi])))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B207C9C4-F54B-43FE-83A4-94948271D532}" name="Berat" dataDxfId="74">
+    <tableColumn id="5" xr3:uid="{B207C9C4-F54B-43FE-83A4-94948271D532}" name="Berat" dataDxfId="67">
       <calculatedColumnFormula>SUM((E70-MIN(Table4[Berat]))/(MAX(Table4[Berat])-MIN(Table4[Berat]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{483EC7A9-DE11-43CA-AA8B-1B2C62CAE18E}" name="Build" dataDxfId="73">
+    <tableColumn id="6" xr3:uid="{483EC7A9-DE11-43CA-AA8B-1B2C62CAE18E}" name="Build" dataDxfId="66">
       <calculatedColumnFormula>SUM((F70-MIN(Table4[Build]))/(MAX(Table4[Build])-MIN(Table4[Build]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{950130C3-E782-4882-9723-18303D45490A}" name="Type Layar" dataDxfId="72">
+    <tableColumn id="7" xr3:uid="{950130C3-E782-4882-9723-18303D45490A}" name="Type Layar" dataDxfId="65">
       <calculatedColumnFormula>SUM((G70-MIN(Table4[Type Layar]))/(MAX(Table4[Type Layar])-MIN(Table4[Type Layar]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E2936121-F44C-4186-B5E8-0449FA00B386}" name="Ukuran Layar" dataDxfId="71">
+    <tableColumn id="8" xr3:uid="{E2936121-F44C-4186-B5E8-0449FA00B386}" name="Ukuran Layar" dataDxfId="64">
       <calculatedColumnFormula>SUM((H70-MIN(Table4[Ukuran Layar]))/(MAX(Table4[Ukuran Layar])-MIN(Table4[Ukuran Layar]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{269AF731-F260-44A0-A781-5617B28E58BB}" name="Resolusi" dataDxfId="70">
+    <tableColumn id="9" xr3:uid="{269AF731-F260-44A0-A781-5617B28E58BB}" name="Resolusi" dataDxfId="63">
       <calculatedColumnFormula>SUM((I70-MIN(Table4[Resolusi]))/(MAX(Table4[Resolusi])-MIN(Table4[Resolusi]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{21FDF078-7A9B-4958-A200-885CCD67988D}" name="OS" dataDxfId="69">
+    <tableColumn id="10" xr3:uid="{21FDF078-7A9B-4958-A200-885CCD67988D}" name="OS" dataDxfId="62">
       <calculatedColumnFormula>SUM((J70-MIN(Table4[OS]))/(MAX(Table4[OS])-MIN(Table4[OS]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{05CC7353-2E07-492E-B34F-C2ACE78447BB}" name="Chipset" dataDxfId="68">
+    <tableColumn id="11" xr3:uid="{05CC7353-2E07-492E-B34F-C2ACE78447BB}" name="Chipset" dataDxfId="61">
       <calculatedColumnFormula>SUM((K70-MIN(Table4[Chipset]))/(MAX(Table4[Chipset])-MIN(Table4[Chipset]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36A175ED-F30A-4DAF-B3ED-7C6D32B3874F}" name="CPU" dataDxfId="67">
+    <tableColumn id="12" xr3:uid="{36A175ED-F30A-4DAF-B3ED-7C6D32B3874F}" name="CPU" dataDxfId="60">
       <calculatedColumnFormula>SUM((L70-MIN(Table4[CPU]))/(MAX(Table4[CPU])-MIN(Table4[CPU]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3094D51B-8022-4E7F-89C1-D80B72F1D173}" name="RAM" dataDxfId="66">
+    <tableColumn id="13" xr3:uid="{3094D51B-8022-4E7F-89C1-D80B72F1D173}" name="RAM" dataDxfId="59">
       <calculatedColumnFormula>SUM((M70-MIN(Table4[RAM]))/(MAX(Table4[RAM])-MIN(Table4[RAM]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{31E589E1-8796-4016-97FB-5C9A014D453F}" name="ROM" dataDxfId="65">
+    <tableColumn id="14" xr3:uid="{31E589E1-8796-4016-97FB-5C9A014D453F}" name="ROM" dataDxfId="58">
       <calculatedColumnFormula>SUM((N70-MIN(Table4[ROM]))/(MAX(Table4[ROM])-MIN(Table4[ROM]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{704ACD05-9693-48E0-896A-594CF1F0AC94}" name="MP Main" dataDxfId="64">
+    <tableColumn id="15" xr3:uid="{704ACD05-9693-48E0-896A-594CF1F0AC94}" name="MP Main" dataDxfId="57">
       <calculatedColumnFormula>SUM((O70-MIN(Table4[MP Main]))/(MAX(Table4[MP Main])-MIN(Table4[MP Main]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{68B7DF8C-F82C-4977-B009-7C5CF83D005C}" name="Tipe Main" dataDxfId="63">
+    <tableColumn id="16" xr3:uid="{68B7DF8C-F82C-4977-B009-7C5CF83D005C}" name="Tipe Main" dataDxfId="56">
       <calculatedColumnFormula>SUM((P70-MIN(Table4[Tipe Main]))/(MAX(Table4[Tipe Main])-MIN(Table4[Tipe Main]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A292189E-C538-41EB-B8D3-BB0416B7413A}" name="Video Main" dataDxfId="62">
+    <tableColumn id="17" xr3:uid="{A292189E-C538-41EB-B8D3-BB0416B7413A}" name="Video Main" dataDxfId="55">
       <calculatedColumnFormula>SUM((Q70-MIN(Table4[Video Main]))/(MAX(Table4[Video Main])-MIN(Table4[Video Main]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{247FC9F1-A915-4DA6-8E56-E46C1C348027}" name="MP Front" dataDxfId="61">
+    <tableColumn id="18" xr3:uid="{247FC9F1-A915-4DA6-8E56-E46C1C348027}" name="MP Front" dataDxfId="54">
       <calculatedColumnFormula>SUM((R70-MIN(Table4[MP Front]))/(MAX(Table4[MP Front])-MIN(Table4[MP Front]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{F9C73FD5-A041-480F-88E9-579575A4F0F5}" name="Video Front" dataDxfId="60">
+    <tableColumn id="19" xr3:uid="{F9C73FD5-A041-480F-88E9-579575A4F0F5}" name="Video Front" dataDxfId="53">
       <calculatedColumnFormula>SUM((S70-MIN(Table4[Video Front]))/(MAX(Table4[Video Front])-MIN(Table4[Video Front]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{52815383-CBBF-413D-B90E-5B62FCD10864}" name="USB Type" dataDxfId="59">
+    <tableColumn id="20" xr3:uid="{52815383-CBBF-413D-B90E-5B62FCD10864}" name="USB Type" dataDxfId="52">
       <calculatedColumnFormula>SUM((T70-MIN(Table4[USB Type]))/(MAX(Table4[USB Type])-MIN(Table4[USB Type]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{AB25EB15-A496-499C-8E3C-E3B2B2C83EAD}" name="Capacity" dataDxfId="58">
+    <tableColumn id="21" xr3:uid="{AB25EB15-A496-499C-8E3C-E3B2B2C83EAD}" name="Capacity" dataDxfId="51">
       <calculatedColumnFormula>SUM((U70-MIN(Table4[Capacity]))/(MAX(Table4[Capacity])-MIN(Table4[Capacity]))*100%)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{5EE3FC42-8182-4791-825D-920142E48974}" name="Harga" dataDxfId="57">
+    <tableColumn id="22" xr3:uid="{5EE3FC42-8182-4791-825D-920142E48974}" name="Harga" dataDxfId="50">
       <calculatedColumnFormula>SUM((MAX(Table4[Harga])-V70)/(MAX(Table4[Harga])-MIN(Table4[Harga]))*100%)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5449,13 +5545,13 @@
   <autoFilter ref="B171:F199" xr:uid="{6D938535-FA74-4082-8909-7E404CD219FD}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{37A55DA0-2B59-409E-B78B-CD21168CA95B}" name="No"/>
-    <tableColumn id="2" xr3:uid="{246E7506-2DD0-42F6-9733-2E13D3F8FBBC}" name="Merek" dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{246E7506-2DD0-42F6-9733-2E13D3F8FBBC}" name="Merek" dataDxfId="49">
       <calculatedColumnFormula>C139</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C72A5643-FD78-48BB-94F2-729F02A0FAE1}" name="Nilai" dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{C72A5643-FD78-48BB-94F2-729F02A0FAE1}" name="Nilai" dataDxfId="48">
       <calculatedColumnFormula>W139</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9CCCB0E5-E1DA-445B-BC71-025511D92F28}" name="Rank" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{9CCCB0E5-E1DA-445B-BC71-025511D92F28}" name="Rank" dataDxfId="47">
       <calculatedColumnFormula>_xlfn.RANK.EQ(Table8[[#This Row],[Nilai]],Table8[Nilai])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{686E8CE0-3C8C-473D-8C77-EF74CC8F17F9}" name="Persentase" dataCellStyle="Percent">
@@ -5467,74 +5563,74 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{71BB11C9-E9A4-4BAC-AEC0-61E5C577625C}" name="Table6" displayName="Table6" ref="A138:W166" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{71BB11C9-E9A4-4BAC-AEC0-61E5C577625C}" name="Table6" displayName="Table6" ref="A138:W166" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="A138:W166" xr:uid="{FF301026-5852-4EA8-8CB4-C4B37CF66C25}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{B9EC439C-1217-4D09-83C9-99EA53FE0D19}" name="No"/>
-    <tableColumn id="2" xr3:uid="{E25DDB2B-3148-4425-8ABF-08187023D540}" name="Brand" dataDxfId="50">
+    <tableColumn id="2" xr3:uid="{E25DDB2B-3148-4425-8ABF-08187023D540}" name="Brand" dataDxfId="43">
       <calculatedColumnFormula>SUM(B108*Bobot!$F$6)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F673BF9E-9E6E-4621-BEDE-BCDC44E1ECEF}" name="Merek">
       <calculatedColumnFormula>C108</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{06507492-B50F-4E0A-870A-10D25BA107B5}" name="Dimensi" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{06507492-B50F-4E0A-870A-10D25BA107B5}" name="Dimensi" dataDxfId="42">
       <calculatedColumnFormula>SUM(D108*Bobot!$F$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{270DC85A-3812-4EA4-94C6-3D051E55DD95}" name="Berat" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{270DC85A-3812-4EA4-94C6-3D051E55DD95}" name="Berat" dataDxfId="41">
       <calculatedColumnFormula>SUM(E108*Bobot!$F$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F99B09EE-82A1-49E2-BDE5-D3F719E85BCB}" name="Build" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{F99B09EE-82A1-49E2-BDE5-D3F719E85BCB}" name="Build" dataDxfId="40">
       <calculatedColumnFormula>SUM(F108*Bobot!$F$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D26DE414-8779-40FA-8057-4C06E4873ADB}" name="Type Layar" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{D26DE414-8779-40FA-8057-4C06E4873ADB}" name="Type Layar" dataDxfId="39">
       <calculatedColumnFormula>SUM(G108*Bobot!$F$8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B7441901-F8B6-426A-8003-681A78F4AD21}" name="Ukuran Layar" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{B7441901-F8B6-426A-8003-681A78F4AD21}" name="Ukuran Layar" dataDxfId="38">
       <calculatedColumnFormula>SUM(H108*Bobot!$F$8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3245CD4C-44A6-40AD-8F86-E11130C7D687}" name="Resolusi" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{3245CD4C-44A6-40AD-8F86-E11130C7D687}" name="Resolusi" dataDxfId="37">
       <calculatedColumnFormula>SUM(I108*Bobot!$F$8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{918894BC-716D-4D9D-82E9-08990A81D257}" name="OS" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{918894BC-716D-4D9D-82E9-08990A81D257}" name="OS" dataDxfId="36">
       <calculatedColumnFormula>SUM(J108*Bobot!$F$9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{6A2F0B58-BB0B-4199-B697-936EE8EA1D6E}" name="Chipset" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{6A2F0B58-BB0B-4199-B697-936EE8EA1D6E}" name="Chipset" dataDxfId="35">
       <calculatedColumnFormula>SUM(K108*Bobot!$F$9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{043D1089-2C04-4C9F-BEBE-728D11230279}" name="CPU" dataDxfId="41">
+    <tableColumn id="12" xr3:uid="{043D1089-2C04-4C9F-BEBE-728D11230279}" name="CPU" dataDxfId="34">
       <calculatedColumnFormula>SUM(L108*Bobot!$F$9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9FD76949-338E-440C-A380-D6F0F0CCBA2E}" name="RAM" dataDxfId="40">
+    <tableColumn id="13" xr3:uid="{9FD76949-338E-440C-A380-D6F0F0CCBA2E}" name="RAM" dataDxfId="33">
       <calculatedColumnFormula>SUM(M108*Bobot!$F$10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6BABFA04-5255-47A6-B15D-5D6C4EBD448A}" name="ROM" dataDxfId="39">
+    <tableColumn id="14" xr3:uid="{6BABFA04-5255-47A6-B15D-5D6C4EBD448A}" name="ROM" dataDxfId="32">
       <calculatedColumnFormula>SUM(N108*Bobot!$F$10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{96D1D0ED-11E8-48E2-B720-59C376CEF59A}" name="MP Main" dataDxfId="38">
+    <tableColumn id="15" xr3:uid="{96D1D0ED-11E8-48E2-B720-59C376CEF59A}" name="MP Main" dataDxfId="31">
       <calculatedColumnFormula>SUM(O108*Bobot!$F$11)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{D617EABD-A264-4FB7-B6E2-15A1D29CBBB1}" name="Tipe Main" dataDxfId="37">
+    <tableColumn id="16" xr3:uid="{D617EABD-A264-4FB7-B6E2-15A1D29CBBB1}" name="Tipe Main" dataDxfId="30">
       <calculatedColumnFormula>SUM(P108*Bobot!$F$11)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{265E020F-CD35-469A-AAB4-01C7CF9D8239}" name="Video Main" dataDxfId="36">
+    <tableColumn id="17" xr3:uid="{265E020F-CD35-469A-AAB4-01C7CF9D8239}" name="Video Main" dataDxfId="29">
       <calculatedColumnFormula>SUM(Q108*Bobot!$F$11)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{98E4B750-769C-4611-9438-0B03C53A498E}" name="MP Front" dataDxfId="35">
+    <tableColumn id="18" xr3:uid="{98E4B750-769C-4611-9438-0B03C53A498E}" name="MP Front" dataDxfId="28">
       <calculatedColumnFormula>SUM(R108*Bobot!$F$12)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{EE968840-E5B5-443C-B331-C40615DBA724}" name="Video Front" dataDxfId="34">
+    <tableColumn id="19" xr3:uid="{EE968840-E5B5-443C-B331-C40615DBA724}" name="Video Front" dataDxfId="27">
       <calculatedColumnFormula>SUM(S108*Bobot!$F$12)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{EC6835A7-099F-43ED-AC92-0499B2D26FEC}" name="USB Type" dataDxfId="33">
+    <tableColumn id="20" xr3:uid="{EC6835A7-099F-43ED-AC92-0499B2D26FEC}" name="USB Type" dataDxfId="26">
       <calculatedColumnFormula>SUM(T108*Bobot!$F$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{09B13E8E-F601-4183-BCEA-B3D2BA19AE7D}" name="Capacity" dataDxfId="32">
+    <tableColumn id="21" xr3:uid="{09B13E8E-F601-4183-BCEA-B3D2BA19AE7D}" name="Capacity" dataDxfId="25">
       <calculatedColumnFormula>SUM(U108*Bobot!$F$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{3F5A54AD-9707-47A0-9921-9B58404E673C}" name="Harga" dataDxfId="31">
+    <tableColumn id="22" xr3:uid="{3F5A54AD-9707-47A0-9921-9B58404E673C}" name="Harga" dataDxfId="24">
       <calculatedColumnFormula>SUM(V108*Bobot!$F$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{9EBEF54B-310F-4F68-BD9A-ADD36E6AF22A}" name="Total" dataDxfId="30">
+    <tableColumn id="23" xr3:uid="{9EBEF54B-310F-4F68-BD9A-ADD36E6AF22A}" name="Total" dataDxfId="23">
       <calculatedColumnFormula>SUM(B139+((D139+E139+F139)/3)+((G139+H139+I139)/3)+((J139+K139+L139)/3)+((M139+N139)/2)+((O139+P139+Q139)/3)+((R139+S139)/2)+((T139+U139)/2)+V139)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5543,71 +5639,71 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF0C14BC-EA5B-4CF5-A556-792A38372F84}" name="Table4" displayName="Table4" ref="A69:V97" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF0C14BC-EA5B-4CF5-A556-792A38372F84}" name="Table4" displayName="Table4" ref="A69:V97" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A69:V97" xr:uid="{AD840710-85CE-413E-A713-BB92CCC6C34B}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{7744EE14-46D9-45E1-886B-617E9C405E33}" name="No"/>
-    <tableColumn id="2" xr3:uid="{1DC42DA3-D002-4196-974F-6792E9A86F8D}" name="Brand" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{1DC42DA3-D002-4196-974F-6792E9A86F8D}" name="Brand" dataDxfId="21">
       <calculatedColumnFormula>B38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{83ED1DE6-CCBD-4467-8AE5-6794F63274FF}" name="Merek" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{83ED1DE6-CCBD-4467-8AE5-6794F63274FF}" name="Merek" dataDxfId="20">
       <calculatedColumnFormula>C38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3DE25371-3535-4E8E-A776-F9AA9F46342A}" name="Dimensi" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{3DE25371-3535-4E8E-A776-F9AA9F46342A}" name="Dimensi" dataDxfId="19">
       <calculatedColumnFormula>IF(D38&lt;=konversi2!$D$8,konversi2!$E$7,IF(D38&lt;=konversi2!$D$10,konversi2!$E$9,IF(D38&lt;=konversi2!$D$15,konversi2!$E$11,IF(D38&lt;=konversi2!$D$19,konversi2!$E$18,IF(D38&lt;=konversi2!$D$21,konversi2!$E$20,IF(D38&gt;konversi2!$D$23,konversi2!$E$22,"kosong"))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B94175EB-762D-4A2F-9E64-2AA052BD0C9F}" name="Berat" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{B94175EB-762D-4A2F-9E64-2AA052BD0C9F}" name="Berat" dataDxfId="18">
       <calculatedColumnFormula>IF(E38&lt;=konversi2!$G$7,konversi2!$H$7,IF(E38&lt;=konversi2!$G$8,konversi2!$H$8,IF(E35&lt;=konversi2!$G$9,konversi2!$H$9,IF(E35&lt;=konversi2!$G$10,konversi2!$H$10,IF(E35&lt;=konversi2!$G$11,konversi2!$H$11,IF(E35&lt;=konversi2!$G$12,konversi2!$H$12,IF(E35&lt;konversi2!$G$13,konversi2!$H$13,IF(E35&gt;=konversi2!$G$13,konversi2!$H$14,"kosong"))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E0C874-1B13-4ECE-9E01-67030AC210DB}" name="Build" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{C2E0C874-1B13-4ECE-9E01-67030AC210DB}" name="Build" dataDxfId="17">
       <calculatedColumnFormula>F38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E9CE02A1-449E-4BAC-AAE8-049F99C6B31A}" name="Type Layar" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{E9CE02A1-449E-4BAC-AAE8-049F99C6B31A}" name="Type Layar" dataDxfId="16">
       <calculatedColumnFormula>G38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D71C8DA-5C0C-44AA-8D3C-231449CAFEA7}" name="Ukuran Layar" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{8D71C8DA-5C0C-44AA-8D3C-231449CAFEA7}" name="Ukuran Layar" dataDxfId="15">
       <calculatedColumnFormula>IF(H38&lt;=konversi2!$L$7,konversi2!$M$7,IF(H38&lt;=konversi2!$L$8,konversi2!$M$8,IF(H38&lt;=konversi2!$L$9,konversi2!$M$9,IF(H38&lt;=konversi2!$L$10,konversi2!$M$10,IF(H38&lt;=konversi2!$L$11,konversi2!$M$11,IF(H38&lt;=konversi2!$L$12,konversi2!$M$12,IF(H38&lt;konversi2!$L$13,konversi2!$M$13,IF(H38&gt;=konversi2!$M$14,0))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{330229BC-2F59-4400-A3A2-C03F9D480422}" name="Resolusi" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{330229BC-2F59-4400-A3A2-C03F9D480422}" name="Resolusi" dataDxfId="14">
       <calculatedColumnFormula>IF(I38&lt;konversi2!$O$7,konversi2!$P$7,IF(I38&lt;konversi2!$O$8,konversi2!$P$8,IF(I38&lt;konversi2!$O$9,konversi2!$P$9,IF(I38&gt;konversi2!$O$10,konversi2!$P$10,"null"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{397791B4-1908-4A4A-8CAC-A7D9A175C191}" name="OS" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{397791B4-1908-4A4A-8CAC-A7D9A175C191}" name="OS" dataDxfId="13">
       <calculatedColumnFormula>J38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{3B5B6DC5-928C-4F92-BD8E-DAD238B9005D}" name="Chipset" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{3B5B6DC5-928C-4F92-BD8E-DAD238B9005D}" name="Chipset" dataDxfId="12">
       <calculatedColumnFormula>K38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{3FD6BD45-6BD8-4AA7-A53D-F1262860048D}" name="CPU" dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{3FD6BD45-6BD8-4AA7-A53D-F1262860048D}" name="CPU" dataDxfId="11">
       <calculatedColumnFormula>L38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{5CBC6A50-F86E-48A7-BC51-1AD2DEFB04D2}" name="RAM" dataDxfId="17">
+    <tableColumn id="13" xr3:uid="{5CBC6A50-F86E-48A7-BC51-1AD2DEFB04D2}" name="RAM" dataDxfId="10">
       <calculatedColumnFormula>IF(M38=konversi2!$Q$7,konversi2!$R$7,IF(M38=konversi2!$Q$8,konversi2!$R$8,IF(M38=konversi2!$Q$9,konversi2!$R$9,"null")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{4D98DCDB-9CAA-401E-8CA2-EC21F1664A9F}" name="ROM" dataDxfId="16">
+    <tableColumn id="14" xr3:uid="{4D98DCDB-9CAA-401E-8CA2-EC21F1664A9F}" name="ROM" dataDxfId="9">
       <calculatedColumnFormula>IF(N38=konversi2!$S$7,konversi2!$T$7,IF(N38=konversi2!$S$8,konversi2!$T$8,IF(N38=konversi2!$S$9,konversi2!$T$9,IF(N38=konversi2!$S$10,konversi2!$T$10,"null"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A8E6F42A-945E-4956-8C6D-F3FE71FB18B7}" name="MP Main" dataDxfId="15">
+    <tableColumn id="15" xr3:uid="{A8E6F42A-945E-4956-8C6D-F3FE71FB18B7}" name="MP Main" dataDxfId="8">
       <calculatedColumnFormula>O38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C71E598B-1FC8-4DE2-81F9-54865BF15135}" name="Tipe Main" dataDxfId="14">
+    <tableColumn id="16" xr3:uid="{C71E598B-1FC8-4DE2-81F9-54865BF15135}" name="Tipe Main" dataDxfId="7">
       <calculatedColumnFormula>P38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{87BD71BA-154F-4EC4-BFEE-5E94D7EF9F97}" name="Video Main" dataDxfId="13">
+    <tableColumn id="17" xr3:uid="{87BD71BA-154F-4EC4-BFEE-5E94D7EF9F97}" name="Video Main" dataDxfId="6">
       <calculatedColumnFormula>perhitungan!Q38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{238B4A59-8844-4452-885E-C5D3ED816038}" name="MP Front" dataDxfId="12">
+    <tableColumn id="18" xr3:uid="{238B4A59-8844-4452-885E-C5D3ED816038}" name="MP Front" dataDxfId="5">
       <calculatedColumnFormula>R38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{B5E3DE4B-2CB2-4ED0-ADD0-9A3A7C3EEF05}" name="Video Front" dataDxfId="11">
+    <tableColumn id="19" xr3:uid="{B5E3DE4B-2CB2-4ED0-ADD0-9A3A7C3EEF05}" name="Video Front" dataDxfId="4">
       <calculatedColumnFormula>S38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{256A1EED-C144-4219-AA49-6DC893086E44}" name="USB Type" dataDxfId="10">
+    <tableColumn id="20" xr3:uid="{256A1EED-C144-4219-AA49-6DC893086E44}" name="USB Type" dataDxfId="3">
       <calculatedColumnFormula>T38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{C5B8BFAC-9A3D-4ED4-804A-2DCF9F4352A7}" name="Capacity" dataDxfId="9">
+    <tableColumn id="21" xr3:uid="{C5B8BFAC-9A3D-4ED4-804A-2DCF9F4352A7}" name="Capacity" dataDxfId="2">
       <calculatedColumnFormula>IF(U38&lt;konversi2!$V$7,konversi2!$W$7,IF(U38&lt;konversi2!$V$8,konversi2!$W$8,IF(U38&lt;konversi2!$V$9,konversi2!$W$9,IF(U38&lt;konversi2!$V$10,konversi2!$W$10,IF(U38&lt;konversi2!$V$11,konversi2!$W$11,IF(U38&gt;=konversi2!$V$12,konversi2!$W$12,"null"))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{E9077B4D-1A15-4FAD-A530-8C5A5B35B034}" name="Harga" dataDxfId="8">
+    <tableColumn id="22" xr3:uid="{E9077B4D-1A15-4FAD-A530-8C5A5B35B034}" name="Harga" dataDxfId="1">
       <calculatedColumnFormula>IF(V38&lt;konversi2!$Y$7,konversi2!$Z$7,IF(V38&lt;konversi2!$Y$8,konversi2!$Z$8,IF(V38&lt;konversi2!$Y$9,konversi2!$Z$9,IF(V38&lt;konversi2!$Y$10,konversi2!$Z$10,IF(V38&lt;konversi2!$Y$11,konversi2!$Z$11,IF(V38&lt;konversi2!$Y$12,konversi2!$Z$12,IF(V38&lt;konversi2!$Y$13,konversi2!$Z$13,IF(V38&gt;=konversi2!$Y$13,konversi2!$Z$14,"null"))))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5620,10 +5716,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="C0C0C0"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="191919"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -5976,18 +6072,18 @@
         <f>C3/SUM(C$3:C$11)</f>
         <v>0.11627906976744186</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="K3" s="74" t="s">
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="K3" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="L3" s="74"/>
-      <c r="N3" s="74" t="s">
+      <c r="L3" s="85"/>
+      <c r="N3" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
@@ -6003,9 +6099,9 @@
         <f t="shared" ref="D4:D11" si="0">C4/SUM(C$3:C$11)</f>
         <v>0.1308139534883721</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
       <c r="R4" t="s">
         <v>202</v>
       </c>
@@ -6026,20 +6122,20 @@
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
-      <c r="M5" s="74" t="s">
+      <c r="M5" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
       <c r="R5" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="S5" s="75" t="s">
+      <c r="S5" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="T5" s="75"/>
+      <c r="T5" s="79"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
@@ -6057,13 +6153,13 @@
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
-      <c r="M6" s="74" t="s">
+      <c r="M6" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
       <c r="R6">
         <f>SUM((100-10)/(100-10)*100%)</f>
         <v>1</v>
@@ -6108,10 +6204,10 @@
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="79" t="s">
         <v>165</v>
       </c>
-      <c r="N8" s="75"/>
+      <c r="N8" s="79"/>
       <c r="R8">
         <f>SUM((10-10)/(100-10)*100%)</f>
         <v>0</v>
@@ -6169,10 +6265,10 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="83" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="77"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="16">
         <f>SUM(C3:C11)</f>
         <v>688</v>
@@ -6181,10 +6277,10 @@
         <f>SUM(D3:D11)</f>
         <v>1</v>
       </c>
-      <c r="M12" s="75" t="s">
+      <c r="M12" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="N12" s="75"/>
+      <c r="N12" s="79"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -6222,11 +6318,11 @@
       </c>
       <c r="T17" s="78"/>
       <c r="U17" s="78"/>
-      <c r="V17" s="79" t="s">
+      <c r="V17" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="W17" s="80"/>
-      <c r="X17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="82"/>
       <c r="Y17" s="2" t="s">
         <v>8</v>
       </c>
@@ -8469,11 +8565,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="M5:Q5"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="S5:T5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="G4:I4"/>
@@ -8481,11 +8577,11 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:L17"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="M5:Q5"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="V17:X17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8551,10 +8647,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="83"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" spans="3:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="20" t="s">
@@ -9041,10 +9137,10 @@
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="85"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="21">
         <f>AVERAGE(E4:E13)</f>
         <v>66.2</v>
@@ -9100,44 +9196,44 @@
       <c r="C18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="D18" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82" t="s">
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82" t="s">
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="82" t="s">
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82" t="s">
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="S18" s="82"/>
-      <c r="T18" s="82"/>
-      <c r="U18" s="82" t="s">
+      <c r="S18" s="87"/>
+      <c r="T18" s="87"/>
+      <c r="U18" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="V18" s="82"/>
-      <c r="W18" s="82"/>
-      <c r="X18" s="82" t="s">
+      <c r="V18" s="87"/>
+      <c r="W18" s="87"/>
+      <c r="X18" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
-      <c r="AA18" s="82"/>
+      <c r="Y18" s="87"/>
+      <c r="Z18" s="87"/>
+      <c r="AA18" s="87"/>
       <c r="AB18" s="24" t="s">
         <v>8</v>
       </c>
@@ -12538,12 +12634,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="C14:D14"/>
     <mergeCell ref="U18:W18"/>
     <mergeCell ref="X18:AA18"/>
     <mergeCell ref="D50:H50"/>
@@ -12554,6 +12644,12 @@
     <mergeCell ref="U50:W50"/>
     <mergeCell ref="X50:AA50"/>
     <mergeCell ref="R18:T18"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -13093,7 +13189,7 @@
       <c r="D7" s="67" t="s">
         <v>285</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="90">
         <v>0</v>
       </c>
       <c r="F7" s="67">
@@ -13161,7 +13257,7 @@
       <c r="D8" s="67">
         <v>80000</v>
       </c>
-      <c r="E8" s="86"/>
+      <c r="E8" s="90"/>
       <c r="F8" s="67">
         <v>168</v>
       </c>
@@ -13227,7 +13323,7 @@
       <c r="D9" s="67">
         <v>80000</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="90">
         <v>20</v>
       </c>
       <c r="F9" s="67">
@@ -13295,7 +13391,7 @@
       <c r="D10" s="67">
         <v>90000</v>
       </c>
-      <c r="E10" s="86"/>
+      <c r="E10" s="90"/>
       <c r="F10" s="67">
         <v>172</v>
       </c>
@@ -13355,7 +13451,7 @@
       <c r="D11" s="67">
         <v>90000</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="90">
         <v>40</v>
       </c>
       <c r="F11" s="67">
@@ -13402,7 +13498,7 @@
       <c r="C12" s="71">
         <v>92632.155000000013</v>
       </c>
-      <c r="E12" s="86"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="67">
         <v>196</v>
       </c>
@@ -13447,7 +13543,7 @@
       <c r="C13" s="71">
         <v>93780.51</v>
       </c>
-      <c r="E13" s="86"/>
+      <c r="E13" s="90"/>
       <c r="F13" s="67">
         <v>201</v>
       </c>
@@ -13486,7 +13582,7 @@
       <c r="C14" s="71">
         <v>97640.555999999997</v>
       </c>
-      <c r="E14" s="86"/>
+      <c r="E14" s="90"/>
       <c r="F14" s="67">
         <v>209</v>
       </c>
@@ -13525,7 +13621,7 @@
       <c r="D15" s="67">
         <v>100000</v>
       </c>
-      <c r="E15" s="86"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="67">
         <v>221</v>
       </c>
@@ -13546,7 +13642,7 @@
       <c r="D16" s="67">
         <v>100000</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="91">
         <v>60</v>
       </c>
       <c r="F16" s="67">
@@ -13566,7 +13662,7 @@
       <c r="D17" s="67">
         <v>110000</v>
       </c>
-      <c r="E17" s="87"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="67">
         <v>234</v>
       </c>
@@ -13584,7 +13680,7 @@
       <c r="D18" s="67">
         <v>110000</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="91">
         <v>80</v>
       </c>
       <c r="F18" s="67">
@@ -13616,7 +13712,7 @@
       <c r="D19" s="67">
         <v>120000</v>
       </c>
-      <c r="E19" s="87"/>
+      <c r="E19" s="91"/>
       <c r="K19" s="67" t="s">
         <v>309</v>
       </c>
@@ -13683,7 +13779,7 @@
       <c r="D22" s="67" t="s">
         <v>286</v>
       </c>
-      <c r="E22" s="86">
+      <c r="E22" s="90">
         <v>100</v>
       </c>
       <c r="K22" s="67" t="s">
@@ -13706,7 +13802,7 @@
       <c r="D23" s="67">
         <v>130000</v>
       </c>
-      <c r="E23" s="86"/>
+      <c r="E23" s="90"/>
       <c r="K23" s="67" t="s">
         <v>313</v>
       </c>
@@ -13875,10 +13971,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F608000-14CD-4E34-AF28-C10DC4CA4115}">
-  <dimension ref="C4:L15"/>
+  <dimension ref="C4:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:L14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13887,20 +13983,20 @@
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="90" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="74" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="48" t="s">
         <v>281</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="48"/>
     </row>
-    <row r="5" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="59" t="s">
         <v>9</v>
       </c>
@@ -13913,7 +14009,7 @@
       <c r="F5" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="75" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="59" t="s">
@@ -13925,8 +14021,11 @@
       <c r="L5" s="59" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="59" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="51">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -13940,7 +14039,7 @@
         <f t="shared" ref="F6:F14" si="0">SUM(E6/$E$15)</f>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="I6" s="92">
+      <c r="I6" s="76">
         <v>1</v>
       </c>
       <c r="J6" s="54" t="s">
@@ -13953,8 +14052,12 @@
         <f t="shared" ref="L6:L13" si="1">SUM(K6/$K$14)</f>
         <v>0.10869565217391304</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="94">
+        <f t="shared" ref="M6:M13" si="2">L6</f>
+        <v>0.10869565217391304</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="53">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -13968,7 +14071,7 @@
         <f t="shared" si="0"/>
         <v>0.10638297872340426</v>
       </c>
-      <c r="I7" s="93">
+      <c r="I7" s="77">
         <v>2</v>
       </c>
       <c r="J7" s="57" t="s">
@@ -13981,8 +14084,12 @@
         <f t="shared" si="1"/>
         <v>0.15217391304347827</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="94">
+        <f t="shared" si="2"/>
+        <v>0.15217391304347827</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="56">
         <v>0.125</v>
       </c>
@@ -13996,7 +14103,7 @@
         <f t="shared" si="0"/>
         <v>0.14893617021276595</v>
       </c>
-      <c r="I8" s="92">
+      <c r="I8" s="76">
         <v>3</v>
       </c>
       <c r="J8" s="54" t="s">
@@ -14009,8 +14116,12 @@
         <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="94">
+        <f t="shared" si="2"/>
+        <v>0.17391304347826086</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="53">
         <v>0.16666666666666666</v>
       </c>
@@ -14024,7 +14135,7 @@
         <f t="shared" si="0"/>
         <v>0.1702127659574468</v>
       </c>
-      <c r="I9" s="93">
+      <c r="I9" s="77">
         <v>4</v>
       </c>
       <c r="J9" s="57" t="s">
@@ -14037,8 +14148,12 @@
         <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="94">
+        <f t="shared" si="2"/>
+        <v>0.17391304347826086</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="56">
         <v>0.20833333333333334</v>
       </c>
@@ -14052,7 +14167,7 @@
         <f t="shared" si="0"/>
         <v>0.1702127659574468</v>
       </c>
-      <c r="I10" s="92">
+      <c r="I10" s="76">
         <v>5</v>
       </c>
       <c r="J10" s="54" t="s">
@@ -14065,8 +14180,12 @@
         <f t="shared" si="1"/>
         <v>2.1739130434782608E-2</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="94">
+        <f t="shared" si="2"/>
+        <v>2.1739130434782608E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="53">
         <v>0.25</v>
       </c>
@@ -14080,7 +14199,7 @@
         <f t="shared" si="0"/>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="I11" s="93">
+      <c r="I11" s="77">
         <v>6</v>
       </c>
       <c r="J11" s="57" t="s">
@@ -14093,8 +14212,12 @@
         <f t="shared" si="1"/>
         <v>2.1739130434782608E-2</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="94">
+        <f t="shared" si="2"/>
+        <v>2.1739130434782608E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="56">
         <v>0.29166666666666669</v>
       </c>
@@ -14108,7 +14231,7 @@
         <f t="shared" si="0"/>
         <v>2.1276595744680851E-2</v>
       </c>
-      <c r="I12" s="92">
+      <c r="I12" s="76">
         <v>7</v>
       </c>
       <c r="J12" s="54" t="s">
@@ -14121,8 +14244,12 @@
         <f t="shared" si="1"/>
         <v>0.15217391304347827</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="94">
+        <f t="shared" si="2"/>
+        <v>0.15217391304347827</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="53">
         <v>0.33333333333333331</v>
       </c>
@@ -14136,7 +14263,7 @@
         <f t="shared" si="0"/>
         <v>0.14893617021276595</v>
       </c>
-      <c r="I13" s="93">
+      <c r="I13" s="77">
         <v>8</v>
       </c>
       <c r="J13" s="61" t="s">
@@ -14149,8 +14276,12 @@
         <f t="shared" si="1"/>
         <v>0.19565217391304349</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M13" s="94">
+        <f t="shared" si="2"/>
+        <v>0.19565217391304349</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="60">
         <v>0.375</v>
       </c>
@@ -14164,24 +14295,28 @@
         <f t="shared" si="0"/>
         <v>0.19148936170212766</v>
       </c>
-      <c r="I14" s="88" t="s">
+      <c r="I14" s="95" t="s">
         <v>161</v>
       </c>
-      <c r="J14" s="88"/>
-      <c r="K14" s="48">
+      <c r="J14" s="95"/>
+      <c r="K14" s="96">
         <f>SUM(Table710[Bobot])</f>
         <v>460</v>
       </c>
-      <c r="L14" s="64">
+      <c r="L14" s="97">
         <f>SUM(Table710[Normalisasi])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="88" t="s">
+      <c r="M14" s="98">
+        <f>SUM(Table710[Bobot Akhir])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="92" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="88"/>
+      <c r="D15" s="92"/>
       <c r="E15" s="48">
         <f>SUM(Table7[Bobot])</f>
         <v>470</v>
@@ -14271,11 +14406,11 @@
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="33"/>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="92" t="s">
         <v>276</v>
       </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -16989,10 +17124,10 @@
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="92" t="s">
         <v>275</v>
       </c>
-      <c r="D36" s="88"/>
+      <c r="D36" s="92"/>
       <c r="P36" t="s">
         <v>5</v>
       </c>
@@ -19558,11 +19693,11 @@
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B68" s="89" t="s">
+      <c r="B68" s="93" t="s">
         <v>293</v>
       </c>
-      <c r="C68" s="89"/>
-      <c r="D68" s="89"/>
+      <c r="C68" s="93"/>
+      <c r="D68" s="93"/>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -24690,10 +24825,10 @@
       </c>
     </row>
     <row r="137" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B137" s="88" t="s">
+      <c r="B137" s="92" t="s">
         <v>277</v>
       </c>
-      <c r="C137" s="88"/>
+      <c r="C137" s="92"/>
     </row>
     <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" s="49" t="s">

</xml_diff>